<commit_message>
More offer in offers.json
</commit_message>
<xml_diff>
--- a/excel/PCoptimum.xlsx
+++ b/excel/PCoptimum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Document\GitHub\pcoptimum_html\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7962D9F-A899-4B84-A0BA-62D6A76A412D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD0A703-31C0-4249-BCA0-BBB080749589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23835" yWindow="7170" windowWidth="13695" windowHeight="12885" xr2:uid="{7A0B6E75-F037-4864-A362-1873AE88B937}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Offers</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>no name Canned Chicken or Beef Broth</t>
+  </si>
+  <si>
+    <t>PC Pork Ribs</t>
+  </si>
+  <si>
+    <t>L Extra Camembert</t>
   </si>
 </sst>
 </file>
@@ -228,13 +234,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478E9977-F543-4674-99C4-7906B4BDCCDB}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,30 +698,27 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>600</v>
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -725,7 +729,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -736,7 +740,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -747,82 +751,82 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>800</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <v>3</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -833,51 +837,51 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>400</v>
+        <v>600</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>600</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -887,71 +891,71 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C32" s="3">
         <v>600</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
-        <v>9</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1800</v>
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C34" s="4">
-        <v>1600</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>800</v>
+        <v>8</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1600</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <v>400</v>
+        <v>800</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
@@ -962,7 +966,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B38" s="1">
         <v>2</v>
@@ -973,84 +977,81 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1">
-        <v>6</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1200</v>
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="1">
-        <v>2</v>
-      </c>
-      <c r="C42">
-        <v>400</v>
+      <c r="A42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="6">
+        <v>2200</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>200</v>
+        <v>6</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1200</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -1060,28 +1061,50 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3">
-        <v>600</v>
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B50" s="1">
         <v>3</v>
       </c>
-      <c r="C48">
+      <c r="C50">
         <v>600</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C48">
-    <sortCondition ref="A2:A48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C50">
+    <sortCondition ref="A1:A50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>